<commit_message>
turbidity bug in google docs corrected
</commit_message>
<xml_diff>
--- a/calib/Calibration.xlsx
+++ b/calib/Calibration.xlsx
@@ -323,6 +323,30 @@
     <xf numFmtId="1" fontId="5" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="5" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="4" borderId="6" xfId="6" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -340,30 +364,6 @@
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="5" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="5" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="4" borderId="6" xfId="6" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -421,9 +421,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.1377379252453472"/>
-          <c:y val="0.16953330415535361"/>
-          <c:w val="0.802067147856518"/>
-          <c:h val="0.66224735998823903"/>
+          <c:y val="0.13180657243895566"/>
+          <c:w val="0.81047018481099953"/>
+          <c:h val="0.69997412269670545"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -604,11 +604,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="51559040"/>
-        <c:axId val="51557504"/>
+        <c:axId val="79430784"/>
+        <c:axId val="79432704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="51559040"/>
+        <c:axId val="79430784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32768"/>
@@ -646,12 +646,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51557504"/>
+        <c:crossAx val="79432704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="51557504"/>
+        <c:axId val="79432704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -699,7 +699,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51559040"/>
+        <c:crossAx val="79430784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1054,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,380 +1070,380 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="18">
+      <c r="B2" s="12">
         <v>400</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="20"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="15"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="16">
+      <c r="A6" s="10">
         <v>0.1</v>
       </c>
       <c r="B6" s="1">
         <f>A6</f>
         <v>0.1</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="13">
         <v>24971</v>
       </c>
       <c r="D6" s="1">
-        <f>B6*1000/400</f>
+        <f t="shared" ref="D6:D24" si="0">B6*1000/400</f>
         <v>0.25</v>
       </c>
-      <c r="E6" s="14"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="16">
+      <c r="A7" s="10">
         <v>0.1</v>
       </c>
       <c r="B7" s="1">
-        <f>B6+A7</f>
+        <f t="shared" ref="B7:B24" si="1">B6+A7</f>
         <v>0.2</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="13">
         <v>23000</v>
       </c>
       <c r="D7" s="1">
-        <f>B7*1000/400</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="E7" s="14"/>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="16">
+      <c r="A8" s="10">
         <v>0.1</v>
       </c>
       <c r="B8" s="1">
-        <f>B7+A8</f>
+        <f t="shared" si="1"/>
         <v>0.30000000000000004</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="13">
         <v>21030</v>
       </c>
       <c r="D8" s="1">
-        <f>B8*1000/400</f>
+        <f t="shared" si="0"/>
         <v>0.75000000000000011</v>
       </c>
-      <c r="E8" s="14"/>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="16">
+      <c r="A9" s="10">
         <v>0.1</v>
       </c>
       <c r="B9" s="1">
-        <f>B8+A9</f>
+        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="13">
         <v>18900</v>
       </c>
       <c r="D9" s="1">
-        <f>B9*1000/400</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E9" s="14"/>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
+      <c r="A10" s="10">
         <v>0.2</v>
       </c>
       <c r="B10" s="1">
-        <f>B9+A10</f>
+        <f t="shared" si="1"/>
         <v>0.60000000000000009</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="13">
         <f>(17190+17164+16962+17092)/4</f>
         <v>17102</v>
       </c>
       <c r="D10" s="1">
-        <f>B10*1000/400</f>
+        <f t="shared" si="0"/>
         <v>1.5000000000000002</v>
       </c>
-      <c r="E10" s="14"/>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
+      <c r="A11" s="10">
         <v>0.2</v>
       </c>
       <c r="B11" s="1">
-        <f>B10+A11</f>
+        <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="13">
         <f>AVERAGE(15931,15525,15646,15700,15887)</f>
         <v>15737.8</v>
       </c>
       <c r="D11" s="1">
-        <f>B11*1000/400</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E11" s="14"/>
+      <c r="E11" s="8"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
+      <c r="A12" s="10">
         <v>0.2</v>
       </c>
       <c r="B12" s="1">
-        <f>B11+A12</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="13">
         <f>AVERAGE(14338,14923,14497,14826,14165,14004)</f>
         <v>14458.833333333334</v>
       </c>
       <c r="D12" s="1">
-        <f>B12*1000/400</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="E12" s="14"/>
+      <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="16">
+      <c r="A13" s="10">
         <v>0.4</v>
       </c>
       <c r="B13" s="1">
-        <f>B12+A13</f>
+        <f t="shared" si="1"/>
         <v>1.4</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="13">
         <f>AVERAGE(12271,12076,11432,12390,11981,11883,11509)</f>
         <v>11934.571428571429</v>
       </c>
       <c r="D13" s="1">
-        <f>B13*1000/400</f>
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="E13" s="14"/>
+      <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="16">
+      <c r="A14" s="10">
         <v>0.4</v>
       </c>
       <c r="B14" s="1">
-        <f>B13+A14</f>
+        <f t="shared" si="1"/>
         <v>1.7999999999999998</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="13">
         <f>AVERAGE(10493,10032,10434,10142,9794,9782,9881,10178)</f>
         <v>10092</v>
       </c>
       <c r="D14" s="1">
-        <f>B14*1000/400</f>
+        <f t="shared" si="0"/>
         <v>4.4999999999999991</v>
       </c>
-      <c r="E14" s="14"/>
+      <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="16">
+      <c r="A15" s="10">
         <v>0.4</v>
       </c>
       <c r="B15" s="1">
-        <f>B14+A15</f>
+        <f t="shared" si="1"/>
         <v>2.1999999999999997</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C15" s="13">
         <f>AVERAGE(8157,8402,7866,8100,7800,8036)</f>
         <v>8060.166666666667</v>
       </c>
       <c r="D15" s="1">
-        <f>B15*1000/400</f>
+        <f t="shared" si="0"/>
         <v>5.4999999999999991</v>
       </c>
-      <c r="E15" s="14"/>
+      <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="16">
+      <c r="A16" s="10">
         <v>0.4</v>
       </c>
       <c r="B16" s="1">
-        <f>B15+A16</f>
+        <f t="shared" si="1"/>
         <v>2.5999999999999996</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16" s="13">
         <f>AVERAGE(7202,7003,6497,6375,6374,6352,6649)</f>
         <v>6636</v>
       </c>
       <c r="D16" s="1">
-        <f>B16*1000/400</f>
+        <f t="shared" si="0"/>
         <v>6.4999999999999991</v>
       </c>
-      <c r="E16" s="14"/>
+      <c r="E16" s="8"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="16">
+      <c r="A17" s="10">
         <v>0.4</v>
       </c>
       <c r="B17" s="1">
-        <f>B16+A17</f>
+        <f t="shared" si="1"/>
         <v>2.9999999999999996</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="13">
         <f>AVERAGE(5746,5369,5286,5464,5708,5385)</f>
         <v>5493</v>
       </c>
       <c r="D17" s="1">
-        <f>B17*1000/400</f>
+        <f t="shared" si="0"/>
         <v>7.4999999999999991</v>
       </c>
-      <c r="E17" s="14"/>
+      <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="16">
+      <c r="A18" s="10">
         <v>0.5</v>
       </c>
       <c r="B18" s="1">
-        <f>B17+A18</f>
+        <f t="shared" si="1"/>
         <v>3.4999999999999996</v>
       </c>
-      <c r="C18" s="19">
+      <c r="C18" s="13">
         <f>AVERAGE(4210,4056,3922,4070,4238,3933)</f>
         <v>4071.5</v>
       </c>
       <c r="D18" s="1">
-        <f>B18*1000/400</f>
+        <f t="shared" si="0"/>
         <v>8.7499999999999982</v>
       </c>
-      <c r="E18" s="14"/>
+      <c r="E18" s="8"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="16">
+      <c r="A19" s="10">
         <v>0.5</v>
       </c>
       <c r="B19" s="1">
-        <f>B18+A19</f>
+        <f t="shared" si="1"/>
         <v>3.9999999999999996</v>
       </c>
-      <c r="C19" s="19">
+      <c r="C19" s="13">
         <f>AVERAGE(3560,3541,3434,3386,3307,3326)</f>
         <v>3425.6666666666665</v>
       </c>
       <c r="D19" s="1">
-        <f>B19*1000/400</f>
+        <f t="shared" si="0"/>
         <v>9.9999999999999982</v>
       </c>
-      <c r="E19" s="14"/>
+      <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="16">
+      <c r="A20" s="10">
         <v>0.5</v>
       </c>
       <c r="B20" s="1">
-        <f>B19+A20</f>
+        <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="13">
         <f>AVERAGE(2722,2604,2738,2603,2574,2492,2521)</f>
         <v>2607.7142857142858</v>
       </c>
       <c r="D20" s="1">
-        <f>B20*1000/400</f>
+        <f t="shared" si="0"/>
         <v>11.25</v>
       </c>
-      <c r="E20" s="14"/>
+      <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="16">
+      <c r="A21" s="10">
         <v>0.5</v>
       </c>
       <c r="B21" s="1">
-        <f>B20+A21</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="C21" s="19">
+      <c r="C21" s="13">
         <f>AVERAGE(2074,2109,2118,2166,2058)</f>
         <v>2105</v>
       </c>
       <c r="D21" s="1">
-        <f>B21*1000/400</f>
+        <f t="shared" si="0"/>
         <v>12.5</v>
       </c>
-      <c r="E21" s="14"/>
+      <c r="E21" s="8"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="16">
+      <c r="A22" s="10">
         <v>0.5</v>
       </c>
       <c r="B22" s="1">
-        <f>B21+A22</f>
+        <f t="shared" si="1"/>
         <v>5.5</v>
       </c>
-      <c r="C22" s="19">
+      <c r="C22" s="13">
         <f>AVERAGE(1493,1589,1548,1587,1527)</f>
         <v>1548.8</v>
       </c>
       <c r="D22" s="1">
-        <f>B22*1000/400</f>
+        <f t="shared" si="0"/>
         <v>13.75</v>
       </c>
-      <c r="E22" s="14"/>
+      <c r="E22" s="8"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="16">
+      <c r="A23" s="10">
         <v>0.5</v>
       </c>
       <c r="B23" s="1">
-        <f>B22+A23</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="C23" s="19">
+      <c r="C23" s="13">
         <f>AVERAGE(1287,1293,1403,1343,1344)</f>
         <v>1334</v>
       </c>
       <c r="D23" s="1">
-        <f>B23*1000/400</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="E23" s="14"/>
+      <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="16">
+      <c r="A24" s="10">
         <v>1</v>
       </c>
       <c r="B24" s="1">
-        <f>B23+A24</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="C24" s="19">
+      <c r="C24" s="13">
         <f>AVERAGE(828,910,882,857,951,942)</f>
         <v>895</v>
       </c>
       <c r="D24" s="1">
-        <f>B24*1000/400</f>
+        <f t="shared" si="0"/>
         <v>17.5</v>
       </c>
-      <c r="E24" s="14"/>
+      <c r="E24" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1519,11 +1519,11 @@
     </row>
     <row r="4" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
-      <c r="B4" s="8" t="e">
+      <c r="B4" s="16" t="e">
         <f>#REF!*0.145</f>
         <v>#REF!</v>
       </c>
-      <c r="C4" s="11" t="e">
+      <c r="C4" s="19" t="e">
         <f>#REF!*101.97162129779</f>
         <v>#REF!</v>
       </c>
@@ -1538,8 +1538,8 @@
     </row>
     <row r="5" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="12"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -1551,8 +1551,8 @@
     </row>
     <row r="6" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="13"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="21"/>
       <c r="D6" s="7"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -1564,11 +1564,11 @@
     </row>
     <row r="7" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
-      <c r="B7" s="8" t="e">
+      <c r="B7" s="16" t="e">
         <f>#REF!*0.145</f>
         <v>#REF!</v>
       </c>
-      <c r="C7" s="11" t="e">
+      <c r="C7" s="19" t="e">
         <f>#REF!*101.97162129779</f>
         <v>#REF!</v>
       </c>
@@ -1583,8 +1583,8 @@
     </row>
     <row r="8" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="12"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -1596,8 +1596,8 @@
     </row>
     <row r="9" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="13"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="21"/>
       <c r="D9" s="7"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -1609,11 +1609,11 @@
     </row>
     <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
-      <c r="B10" s="8" t="e">
+      <c r="B10" s="16" t="e">
         <f>#REF!*0.145</f>
         <v>#REF!</v>
       </c>
-      <c r="C10" s="11" t="e">
+      <c r="C10" s="19" t="e">
         <f>#REF!*101.97162129779</f>
         <v>#REF!</v>
       </c>
@@ -1628,8 +1628,8 @@
     </row>
     <row r="11" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="12"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="7"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -1641,8 +1641,8 @@
     </row>
     <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="13"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="21"/>
       <c r="D12" s="7"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
@@ -1654,11 +1654,11 @@
     </row>
     <row r="13" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
-      <c r="B13" s="8" t="e">
+      <c r="B13" s="16" t="e">
         <f>#REF!*0.145</f>
         <v>#REF!</v>
       </c>
-      <c r="C13" s="11" t="e">
+      <c r="C13" s="19" t="e">
         <f>#REF!*101.97162129779</f>
         <v>#REF!</v>
       </c>
@@ -1673,8 +1673,8 @@
     </row>
     <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="12"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="7"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -1686,8 +1686,8 @@
     </row>
     <row r="15" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="13"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="21"/>
       <c r="D15" s="7"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -1699,11 +1699,11 @@
     </row>
     <row r="16" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
-      <c r="B16" s="8" t="e">
+      <c r="B16" s="16" t="e">
         <f>#REF!*0.145</f>
         <v>#REF!</v>
       </c>
-      <c r="C16" s="11" t="e">
+      <c r="C16" s="19" t="e">
         <f>#REF!*101.97162129779</f>
         <v>#REF!</v>
       </c>
@@ -1718,8 +1718,8 @@
     </row>
     <row r="17" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="12"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="7"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
@@ -1731,8 +1731,8 @@
     </row>
     <row r="18" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="13"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="21"/>
       <c r="D18" s="7"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -1744,11 +1744,11 @@
     </row>
     <row r="19" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
-      <c r="B19" s="8" t="e">
+      <c r="B19" s="16" t="e">
         <f>#REF!*0.145</f>
         <v>#REF!</v>
       </c>
-      <c r="C19" s="11" t="e">
+      <c r="C19" s="19" t="e">
         <f>#REF!*101.97162129779</f>
         <v>#REF!</v>
       </c>
@@ -1763,8 +1763,8 @@
     </row>
     <row r="20" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="12"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="20"/>
       <c r="D20" s="7"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
@@ -1776,8 +1776,8 @@
     </row>
     <row r="21" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="13"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="21"/>
       <c r="D21" s="7"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
@@ -1789,11 +1789,11 @@
     </row>
     <row r="22" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
-      <c r="B22" s="8" t="e">
+      <c r="B22" s="16" t="e">
         <f>#REF!*0.145</f>
         <v>#REF!</v>
       </c>
-      <c r="C22" s="11" t="e">
+      <c r="C22" s="19" t="e">
         <f>#REF!*101.97162129779</f>
         <v>#REF!</v>
       </c>
@@ -1808,8 +1808,8 @@
     </row>
     <row r="23" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="12"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="20"/>
       <c r="D23" s="7"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
@@ -1821,8 +1821,8 @@
     </row>
     <row r="24" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="13"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="21"/>
       <c r="D24" s="7"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
@@ -1860,6 +1860,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="C22:C24"/>
     <mergeCell ref="B13:B15"/>
@@ -1868,12 +1874,6 @@
     <mergeCell ref="C16:C18"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="C19:C21"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
implementation of calibration of turbidity using a txt file
</commit_message>
<xml_diff>
--- a/calib/Calibration.xlsx
+++ b/calib/Calibration.xlsx
@@ -4,17 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="12450" windowHeight="10620"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="12450" windowHeight="10620" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="turbidity" sheetId="1" r:id="rId1"/>
-    <sheet name="pressure" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="turbidity_ODL_#40" sheetId="1" r:id="rId1"/>
+    <sheet name="turbidity_soilTest_#60" sheetId="4" r:id="rId2"/>
+    <sheet name="pressure" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">turbidity!#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'turbidity_ODL_#40'!#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'turbidity_soilTest_#60'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -53,8 +56,92 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Ricardo Neves Correia dos Santos</author>
+  </authors>
+  <commentList>
+    <comment ref="A4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ricardo Neves Correia dos Santos:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+soil passing #40 sieve
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ricardo Neves Correia dos Santos:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+sujidade parasita</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ricardo Neves Correia dos Santos:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+tap water
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>psi</t>
   </si>
@@ -99,6 +186,18 @@
   </si>
   <si>
     <t>water volume used:</t>
+  </si>
+  <si>
+    <t>ln</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Tb=</t>
+  </si>
+  <si>
+    <t>Tb</t>
   </si>
 </sst>
 </file>
@@ -216,7 +315,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -290,6 +389,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -300,7 +455,7 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -346,6 +501,27 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="4" borderId="8" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="4" borderId="10" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -400,7 +576,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -464,7 +639,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>turbidity!$C$6:$C$25</c:f>
+              <c:f>'turbidity_ODL_#40'!$C$6:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="20"/>
@@ -530,7 +705,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>turbidity!$D$6:$D$25</c:f>
+              <c:f>'turbidity_ODL_#40'!$D$6:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -604,11 +779,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="79430784"/>
-        <c:axId val="79432704"/>
+        <c:axId val="40150144"/>
+        <c:axId val="40152064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="79430784"/>
+        <c:axId val="40150144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32768"/>
@@ -646,12 +821,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79432704"/>
+        <c:crossAx val="40152064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="79432704"/>
+        <c:axId val="40152064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -699,7 +874,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79430784"/>
+        <c:crossAx val="40150144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -714,6 +889,534 @@
           <c:y val="0.19790461224366812"/>
           <c:w val="0.47277865266841645"/>
           <c:h val="0.15277748805774002"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Turbidimeter </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Calibration</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.35307830168057441"/>
+          <c:y val="3.3534872636798184E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1377379252453472"/>
+          <c:y val="0.13180657243895566"/>
+          <c:w val="0.81047018481099953"/>
+          <c:h val="0.69997412269670545"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Test_soil</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'turbidity_soilTest_#60'!$C$6:$C$32</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>27603.599999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25595.200000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23722.400000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22490.799999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20808.833333333332</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19433.333333333332</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17197</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15390.375</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13685.222222222223</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12108.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10443.09090909091</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8695.0769230769238</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7080.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5723.9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4666.4666666666662</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4080.7333333333331</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3232</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2591.4375</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2178.818181818182</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1907.8888888888889</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1649.2307692307693</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1309.1818181818182</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1005.4545454545455</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>747</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>620.08333333333337</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>503.90909090909093</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>447.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'turbidity_soilTest_#60'!$D$6:$D$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75000000000000011</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.2499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.7499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.2499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.7499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.7499999999999991</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.7499999999999991</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.7499999999999982</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.9999999999999982</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11.25</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>13.75</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>calib</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="log"/>
+            <c:backward val="10000"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.113563849011001E-2"/>
+                  <c:y val="-0.19709131189345944"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'turbidity_soilTest_#60'!$C$6:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>27603.599999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25595.200000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23722.400000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22490.799999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20808.833333333332</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19433.333333333332</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17197</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15390.375</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13685.222222222223</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12108.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10443.09090909091</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8695.0769230769238</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7080.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5723.9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4666.4666666666662</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'turbidity_soilTest_#60'!$D$6:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75000000000000011</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.2499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.7499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.2499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.7499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.7499999999999991</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.7499999999999991</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="44738048"/>
+        <c:axId val="44739968"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="44738048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="25000"/>
+          <c:min val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t># analog (15bits)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.46414698162729656"/>
+              <c:y val="0.91203703703703709"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="44739968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="44739968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>turbidity (grams/)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.8885931469860125E-2"/>
+              <c:y val="0.31328868002557481"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="44738048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.6576361548323586"/>
+          <c:y val="0.2482069075236279"/>
+          <c:w val="0.28419197842827121"/>
+          <c:h val="0.14858556112489693"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -749,6 +1452,43 @@
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>486757</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>72107</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>175345</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>53789</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1054,8 +1794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1457,6 +2197,597 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:K32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="4" style="1" customWidth="1"/>
+    <col min="9" max="9" width="2.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="12">
+        <v>400</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="F4" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="1">
+        <v>-4.3369999999999997</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="1" t="str">
+        <f>"+"</f>
+        <v>+</v>
+      </c>
+      <c r="K4" s="1">
+        <v>44.155000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="B6" s="15">
+        <f>A6</f>
+        <v>0.05</v>
+      </c>
+      <c r="C6" s="16">
+        <f>AVERAGE(27614,27607,27612,27606,27579)</f>
+        <v>27603.599999999999</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" ref="D6:D25" si="0">B6*1000/400</f>
+        <v>0.125</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="B7" s="1">
+        <f>A7</f>
+        <v>0.1</v>
+      </c>
+      <c r="C7" s="13">
+        <f>AVERAGE(25906,25666,25712,25447,25245)</f>
+        <v>25595.200000000001</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="22">
+        <v>27000</v>
+      </c>
+      <c r="G7" s="1">
+        <f>$G$4*LN(F7)+$K$4</f>
+        <v>-9.797913280630155E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" ref="B8:B25" si="1">B7+A8</f>
+        <v>0.2</v>
+      </c>
+      <c r="C8" s="13">
+        <f>AVERAGE(23600,23873,23971,23514,23654)</f>
+        <v>23722.400000000001</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="22">
+        <v>1900</v>
+      </c>
+      <c r="G8" s="1">
+        <f>$G$4*LN(F8)+$K$4</f>
+        <v>11.412345050724795</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" si="1"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="C9" s="13">
+        <f>AVERAGE(22480,22237,22505,22754,22478)</f>
+        <v>22490.799999999999</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.75000000000000011</v>
+      </c>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="C10" s="13">
+        <f>AVERAGE(21102,20758,20478,20888,21021,20606)</f>
+        <v>20808.833333333332</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="13">
+        <f>AVERAGE(19032,19376,19951,19682,19508,19051)</f>
+        <v>19433.333333333332</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" si="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="C12" s="13">
+        <f>AVERAGE(17443,17133,17403,16980,17281,16942)</f>
+        <v>17197</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>1.75</v>
+      </c>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="B13" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="C13" s="13">
+        <f>AVERAGE(15989,15607,15597,15312,15278,15292,15046,15002)</f>
+        <v>15390.375</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2499999999999996</v>
+      </c>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="B14" s="1">
+        <f t="shared" si="1"/>
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="C14" s="13">
+        <f>AVERAGE(13836,14303,13680,13955,13248,13576,13506,13707,13356)</f>
+        <v>13685.222222222223</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>2.7499999999999996</v>
+      </c>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="B15" s="1">
+        <f t="shared" si="1"/>
+        <v>1.2999999999999998</v>
+      </c>
+      <c r="C15" s="13">
+        <f>AVERAGE(12158,12513,12231,12027,12148,12061,11767,12177,12060,11943)</f>
+        <v>12108.5</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>3.2499999999999996</v>
+      </c>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="B16" s="1">
+        <f t="shared" si="1"/>
+        <v>1.4999999999999998</v>
+      </c>
+      <c r="C16" s="13">
+        <f>AVERAGE(10313,10184,10732,10596,10497,10405,10459,10869,10332,10069,10418)</f>
+        <v>10443.09090909091</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>3.7499999999999996</v>
+      </c>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="B17" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9</v>
+      </c>
+      <c r="C17" s="13">
+        <f>AVERAGE(8555,9041,8820,9041,8848,8723,8393,8738,8371,8452,8506,8805,8743)</f>
+        <v>8695.0769230769238</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>4.75</v>
+      </c>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="B18" s="1">
+        <f t="shared" si="1"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C18" s="13">
+        <f>AVERAGE(7153,7022,7196,6963,7070,7010,7195,7039,7067,7094)</f>
+        <v>7080.9</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>5.75</v>
+      </c>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="B19" s="1">
+        <f t="shared" si="1"/>
+        <v>2.6999999999999997</v>
+      </c>
+      <c r="C19" s="13">
+        <f>AVERAGE(5938,5671,5825,5599,5774,5674,5788,5914,5627,5429)</f>
+        <v>5723.9</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>6.7499999999999991</v>
+      </c>
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="B20" s="1">
+        <f t="shared" si="1"/>
+        <v>3.0999999999999996</v>
+      </c>
+      <c r="C20" s="13">
+        <f>AVERAGE(4855,4774,4804,4702,4467,4844,4589,4791,4686,4650,4606,4559,4569,4597,4504)</f>
+        <v>4666.4666666666662</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>7.7499999999999991</v>
+      </c>
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="B21" s="1">
+        <f t="shared" si="1"/>
+        <v>3.4999999999999996</v>
+      </c>
+      <c r="C21" s="13">
+        <f>AVERAGE(4234,4149,4143,4090,3981,4099,4263,4035,4048,4062,3978,4027,4078,4009,4015)</f>
+        <v>4080.7333333333331</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>8.7499999999999982</v>
+      </c>
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="B22" s="1">
+        <f t="shared" si="1"/>
+        <v>3.9999999999999996</v>
+      </c>
+      <c r="C22" s="13">
+        <f>AVERAGE(3118,3066,3115,2962,3061,2977,3131,2918,2963,3013,3061,3060,2971)+200</f>
+        <v>3232</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999982</v>
+      </c>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="B23" s="1">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+      <c r="C23" s="13">
+        <f>AVERAGE(2624,2574,2630,2543,2458,2464,2526,2494,2605,2698,2543,2597,2390,2472,2533,2512)+50</f>
+        <v>2591.4375</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="0"/>
+        <v>11.25</v>
+      </c>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="B24" s="1">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C24" s="13">
+        <f>AVERAGE(2187,2259,2226,2227,2172,2152,2168,2162,2129,2124,2161)</f>
+        <v>2178.818181818182</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="B25" s="1">
+        <f t="shared" si="1"/>
+        <v>5.5</v>
+      </c>
+      <c r="C25" s="13">
+        <f>AVERAGE(1986,1933,1928,1925,1850,1912,1797,1957,1883)</f>
+        <v>1907.8888888888889</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="0"/>
+        <v>13.75</v>
+      </c>
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="B26" s="20">
+        <f t="shared" ref="B26:B32" si="2">B25+A26</f>
+        <v>6</v>
+      </c>
+      <c r="C26" s="21">
+        <f>AVERAGE(1634,1746,1716,1643,1678,1638,1660,1632,1695,1552,1699,1546,1601)</f>
+        <v>1649.2307692307693</v>
+      </c>
+      <c r="D26" s="20">
+        <f t="shared" ref="D26:D32" si="3">B26*1000/400</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="17">
+        <v>1</v>
+      </c>
+      <c r="B27" s="1">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="C27" s="18">
+        <f>AVERAGE(1383,1364,1305,1322,1337,1296,1305,1269,1255,1275,1290)</f>
+        <v>1309.1818181818182</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="3"/>
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <v>1</v>
+      </c>
+      <c r="B28" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="C28" s="13">
+        <f>AVERAGE(1098,1053,1017,1054,1002,986,1041,951,938,965,955)</f>
+        <v>1005.4545454545455</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
+        <v>2</v>
+      </c>
+      <c r="B29" s="1">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="C29" s="13">
+        <f>AVERAGE(783,757,763,769,755,755,750,757,672,727,729)</f>
+        <v>747</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
+        <v>2</v>
+      </c>
+      <c r="B30" s="1">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="C30" s="13">
+        <f>AVERAGE(617,642,620,638,613,632,599,613,613,621,613,620)</f>
+        <v>620.08333333333337</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="10">
+        <v>2</v>
+      </c>
+      <c r="B31" s="1">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="C31" s="13">
+        <f>AVERAGE(511,507,499,505,498,499,501,510,506,498,509)</f>
+        <v>503.90909090909093</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
+        <v>2</v>
+      </c>
+      <c r="B32" s="1">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="C32" s="13">
+        <f>AVERAGE(467,434,440,450,448,453,451,453,465,434,454,463,449,434,428,437)</f>
+        <v>447.5</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;D</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
@@ -1519,11 +2850,11 @@
     </row>
     <row r="4" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
-      <c r="B4" s="16" t="e">
+      <c r="B4" s="23" t="e">
         <f>#REF!*0.145</f>
         <v>#REF!</v>
       </c>
-      <c r="C4" s="19" t="e">
+      <c r="C4" s="26" t="e">
         <f>#REF!*101.97162129779</f>
         <v>#REF!</v>
       </c>
@@ -1538,8 +2869,8 @@
     </row>
     <row r="5" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="20"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -1551,8 +2882,8 @@
     </row>
     <row r="6" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="21"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="28"/>
       <c r="D6" s="7"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -1564,11 +2895,11 @@
     </row>
     <row r="7" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
-      <c r="B7" s="16" t="e">
+      <c r="B7" s="23" t="e">
         <f>#REF!*0.145</f>
         <v>#REF!</v>
       </c>
-      <c r="C7" s="19" t="e">
+      <c r="C7" s="26" t="e">
         <f>#REF!*101.97162129779</f>
         <v>#REF!</v>
       </c>
@@ -1583,8 +2914,8 @@
     </row>
     <row r="8" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="20"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -1596,8 +2927,8 @@
     </row>
     <row r="9" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="21"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="28"/>
       <c r="D9" s="7"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -1609,11 +2940,11 @@
     </row>
     <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
-      <c r="B10" s="16" t="e">
+      <c r="B10" s="23" t="e">
         <f>#REF!*0.145</f>
         <v>#REF!</v>
       </c>
-      <c r="C10" s="19" t="e">
+      <c r="C10" s="26" t="e">
         <f>#REF!*101.97162129779</f>
         <v>#REF!</v>
       </c>
@@ -1628,8 +2959,8 @@
     </row>
     <row r="11" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="20"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="7"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -1641,8 +2972,8 @@
     </row>
     <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="21"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="28"/>
       <c r="D12" s="7"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
@@ -1654,11 +2985,11 @@
     </row>
     <row r="13" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
-      <c r="B13" s="16" t="e">
+      <c r="B13" s="23" t="e">
         <f>#REF!*0.145</f>
         <v>#REF!</v>
       </c>
-      <c r="C13" s="19" t="e">
+      <c r="C13" s="26" t="e">
         <f>#REF!*101.97162129779</f>
         <v>#REF!</v>
       </c>
@@ -1673,8 +3004,8 @@
     </row>
     <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="20"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="7"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -1686,8 +3017,8 @@
     </row>
     <row r="15" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="21"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="28"/>
       <c r="D15" s="7"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -1699,11 +3030,11 @@
     </row>
     <row r="16" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
-      <c r="B16" s="16" t="e">
+      <c r="B16" s="23" t="e">
         <f>#REF!*0.145</f>
         <v>#REF!</v>
       </c>
-      <c r="C16" s="19" t="e">
+      <c r="C16" s="26" t="e">
         <f>#REF!*101.97162129779</f>
         <v>#REF!</v>
       </c>
@@ -1718,8 +3049,8 @@
     </row>
     <row r="17" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="20"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="27"/>
       <c r="D17" s="7"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
@@ -1731,8 +3062,8 @@
     </row>
     <row r="18" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="21"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="28"/>
       <c r="D18" s="7"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -1744,11 +3075,11 @@
     </row>
     <row r="19" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
-      <c r="B19" s="16" t="e">
+      <c r="B19" s="23" t="e">
         <f>#REF!*0.145</f>
         <v>#REF!</v>
       </c>
-      <c r="C19" s="19" t="e">
+      <c r="C19" s="26" t="e">
         <f>#REF!*101.97162129779</f>
         <v>#REF!</v>
       </c>
@@ -1763,8 +3094,8 @@
     </row>
     <row r="20" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="20"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="7"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
@@ -1776,8 +3107,8 @@
     </row>
     <row r="21" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="21"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="28"/>
       <c r="D21" s="7"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
@@ -1789,11 +3120,11 @@
     </row>
     <row r="22" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
-      <c r="B22" s="16" t="e">
+      <c r="B22" s="23" t="e">
         <f>#REF!*0.145</f>
         <v>#REF!</v>
       </c>
-      <c r="C22" s="19" t="e">
+      <c r="C22" s="26" t="e">
         <f>#REF!*101.97162129779</f>
         <v>#REF!</v>
       </c>
@@ -1808,8 +3139,8 @@
     </row>
     <row r="23" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="20"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="27"/>
       <c r="D23" s="7"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
@@ -1821,8 +3152,8 @@
     </row>
     <row r="24" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="21"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="28"/>
       <c r="D24" s="7"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
@@ -1879,7 +3210,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
put current flow rate in sensors page
</commit_message>
<xml_diff>
--- a/calib/Calibration.xlsx
+++ b/calib/Calibration.xlsx
@@ -141,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>psi</t>
   </si>
@@ -198,6 +198,12 @@
   </si>
   <si>
     <t>Tb</t>
+  </si>
+  <si>
+    <t>analog#</t>
+  </si>
+  <si>
+    <t>turbidity</t>
   </si>
 </sst>
 </file>
@@ -1078,7 +1084,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>0.125</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.25</c:v>
@@ -1166,35 +1172,17 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>calib</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="28575">
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:trendline>
-            <c:trendlineType val="log"/>
-            <c:backward val="10000"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="2.113563849011001E-2"/>
-                  <c:y val="-0.19709131189345944"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'turbidity_soilTest_#60'!$C$6:$C$20</c:f>
+              <c:f>'turbidity_soilTest_#60'!$C$6:$C$32</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>27603.599999999999</c:v>
                 </c:pt>
@@ -1239,18 +1227,54 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>4666.4666666666662</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4080.7333333333331</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3232</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2591.4375</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2178.818181818182</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1907.8888888888889</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1649.2307692307693</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1309.1818181818182</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1005.4545454545455</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>747</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>620.08333333333337</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>503.90909090909093</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>447.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'turbidity_soilTest_#60'!$D$6:$D$20</c:f>
+              <c:f>'turbidity_soilTest_#60'!$D$6:$D$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>0.125</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.25</c:v>
@@ -1293,6 +1317,42 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>7.7499999999999991</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.7499999999999982</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.9999999999999982</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11.25</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>13.75</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2200,8 +2260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2241,7 +2301,9 @@
       <c r="C4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="14"/>
+      <c r="D4" s="14" t="s">
+        <v>20</v>
+      </c>
       <c r="F4" s="22" t="s">
         <v>17</v>
       </c>
@@ -2270,7 +2332,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>6</v>
@@ -2279,11 +2341,11 @@
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="B6" s="15">
         <f>A6</f>
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="C6" s="16">
         <f>AVERAGE(27614,27607,27612,27606,27579)</f>
@@ -2291,7 +2353,7 @@
       </c>
       <c r="D6" s="1">
         <f t="shared" ref="D6:D25" si="0">B6*1000/400</f>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="22" t="s">
@@ -2319,11 +2381,11 @@
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="22">
-        <v>27000</v>
+        <v>27200</v>
       </c>
       <c r="G7" s="1">
         <f>$G$4*LN(F7)+$K$4</f>
-        <v>-9.797913280630155E-2</v>
+        <v>-0.12998665815609201</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>